<commit_message>
Modification on Base template.xlsx and config_parameters.py files.
</commit_message>
<xml_diff>
--- a/source/Base template.xlsx
+++ b/source/Base template.xlsx
@@ -6,14 +6,17 @@
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
-    <sheet name="Network_info" sheetId="2" r:id="rId5"/>
-    <sheet name="Network_parameters" sheetId="3" r:id="rId6"/>
+    <sheet name="Network info" sheetId="2" r:id="rId5"/>
+    <sheet name="ABCD-parameters" sheetId="3" r:id="rId6"/>
+    <sheet name="Z-parameters" sheetId="4" r:id="rId7"/>
+    <sheet name="Y-parameters" sheetId="5" r:id="rId8"/>
+    <sheet name="S-parameters" sheetId="6" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -33,6 +36,31 @@
     <t>Table 1</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="13"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Network_info</t>
+    </r>
+  </si>
+  <si>
+    <t>Network_parameters</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="13"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Network_parameters</t>
+    </r>
+  </si>
+  <si>
     <t>FRECUENCY PARAMETERS</t>
   </si>
   <si>
@@ -54,10 +82,10 @@
     <t>PARAMETERS TO CALCULATE</t>
   </si>
   <si>
-    <t>NETWORKS INFO</t>
-  </si>
-  <si>
-    <t>NETWORK ID</t>
+    <t>SUB-NETWORKS INFO</t>
+  </si>
+  <si>
+    <t>SUB-NETWORK ID</t>
   </si>
   <si>
     <t>CONNECTION TYPE</t>
@@ -87,13 +115,58 @@
     <t>LENGTH</t>
   </si>
   <si>
-    <t>Network_parameters</t>
-  </si>
-  <si>
     <t>PARAMETERS</t>
   </si>
   <si>
-    <t>OPERATION FREQUENCY</t>
+    <t>FREQUENCY</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Z_11</t>
+  </si>
+  <si>
+    <t>Z_12</t>
+  </si>
+  <si>
+    <t>Z_21</t>
+  </si>
+  <si>
+    <t>Z_22</t>
+  </si>
+  <si>
+    <t>Y_11</t>
+  </si>
+  <si>
+    <t>Y_12</t>
+  </si>
+  <si>
+    <t>Y_21</t>
+  </si>
+  <si>
+    <t>Y_22</t>
+  </si>
+  <si>
+    <t>S_11</t>
+  </si>
+  <si>
+    <t>S_12</t>
+  </si>
+  <si>
+    <t>S_21</t>
+  </si>
+  <si>
+    <t>S_22</t>
   </si>
 </sst>
 </file>
@@ -112,6 +185,16 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -120,19 +203,9 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="12"/>
-      <color indexed="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
+      <color indexed="13"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -151,7 +224,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -174,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -184,11 +257,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -197,7 +270,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -205,17 +278,73 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
@@ -236,7 +365,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -301,13 +430,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="8"/>
       </right>
@@ -339,13 +461,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -354,31 +476,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -388,101 +510,155 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -502,13 +678,13 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ff7f7f7f"/>
-      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff4f81bd"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -659,9 +835,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -741,7 +917,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -768,10 +944,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1018,9 +1194,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1298,7 +1474,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1325,10 +1501,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1570,278 +1746,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="30.5547" customWidth="1"/>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="4" width="30.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+    </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+      <c r="A3" s="5"/>
+      <c r="B3" t="s" s="8">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" ht="17.9" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" t="s" s="9">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="9">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" ht="15.35" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" t="s" s="10">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" ht="15.35" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="12"/>
+      <c r="C10" t="s" s="13">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="s" s="3">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4"/>
-      <c r="C12" t="s" s="4">
+      <c r="D10" t="s" s="14">
+        <v>6</v>
+      </c>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" ht="15.35" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s" s="10">
+        <v>7</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" ht="15.35" customHeight="1">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" t="s" s="17">
         <v>5</v>
       </c>
-      <c r="D12" t="s" s="5">
-        <v>24</v>
-      </c>
+      <c r="D12" t="s" s="18">
+        <v>8</v>
+      </c>
+      <c r="E12" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'Network_info'!R1C1" tooltip="" display="Network_info"/>
-    <hyperlink ref="D12" location="'Network_parameters'!R1C1" tooltip="" display="Network_parameters"/>
+    <hyperlink ref="D10" location="'Network info'!R1C1" tooltip="" display="Network_info"/>
+    <hyperlink ref="D12" location="'Z-parameters'!R1C1" tooltip="" display="Network_parameters"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.6719" style="6" customWidth="1"/>
-    <col min="3" max="3" width="11.8516" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.3516" style="6" customWidth="1"/>
-    <col min="5" max="5" width="6.17188" style="6" customWidth="1"/>
-    <col min="6" max="6" width="10.1719" style="6" customWidth="1"/>
-    <col min="7" max="7" width="6.17188" style="6" customWidth="1"/>
-    <col min="8" max="8" width="10.1719" style="6" customWidth="1"/>
-    <col min="9" max="9" width="6.17188" style="6" customWidth="1"/>
-    <col min="10" max="10" width="25.8516" style="6" customWidth="1"/>
-    <col min="11" max="11" width="15.8516" style="6" customWidth="1"/>
-    <col min="12" max="12" width="7.5" style="6" customWidth="1"/>
-    <col min="13" max="16384" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="20" customWidth="1"/>
+    <col min="2" max="2" width="16.6719" style="20" customWidth="1"/>
+    <col min="3" max="3" width="11.8516" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.3516" style="20" customWidth="1"/>
+    <col min="5" max="5" width="6.17188" style="20" customWidth="1"/>
+    <col min="6" max="6" width="10.1719" style="20" customWidth="1"/>
+    <col min="7" max="7" width="6.17188" style="20" customWidth="1"/>
+    <col min="8" max="8" width="10.1719" style="20" customWidth="1"/>
+    <col min="9" max="9" width="6.17188" style="20" customWidth="1"/>
+    <col min="10" max="10" width="25.8516" style="20" customWidth="1"/>
+    <col min="11" max="11" width="15.8516" style="20" customWidth="1"/>
+    <col min="12" max="12" width="7.5" style="20" customWidth="1"/>
+    <col min="13" max="16384" width="8.85156" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="8.5" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="9"/>
+      <c r="A1" t="s" s="21">
+        <v>9</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" ht="8.5" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="12"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="26"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="13">
-        <v>7</v>
-      </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="17"/>
+      <c r="A3" t="s" s="27">
+        <v>10</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="31"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="13">
-        <v>8</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="20"/>
+      <c r="A4" t="s" s="27">
+        <v>11</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="34"/>
     </row>
     <row r="5" ht="43.5" customHeight="1">
-      <c r="A5" t="s" s="21">
-        <v>9</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="24"/>
+      <c r="A5" t="s" s="35">
+        <v>12</v>
+      </c>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="38"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="25">
-        <v>10</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
+      <c r="A6" t="s" s="39">
+        <v>13</v>
+      </c>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="21">
-        <v>11</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="17"/>
+      <c r="A7" t="s" s="35">
+        <v>14</v>
+      </c>
+      <c r="B7" s="36"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="31"/>
     </row>
     <row r="8" ht="29" customHeight="1">
-      <c r="A8" t="s" s="21">
-        <v>12</v>
-      </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="24"/>
+      <c r="A8" t="s" s="35">
+        <v>15</v>
+      </c>
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="38"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" t="s" s="25">
-        <v>13</v>
-      </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
+      <c r="A9" t="s" s="39">
+        <v>16</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" t="s" s="13">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s" s="13">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s" s="13">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s" s="13">
+      <c r="A10" t="s" s="27">
         <v>17</v>
       </c>
-      <c r="E10" t="s" s="13">
+      <c r="B10" t="s" s="27">
         <v>18</v>
       </c>
-      <c r="F10" t="s" s="13">
+      <c r="C10" t="s" s="27">
         <v>19</v>
       </c>
-      <c r="G10" t="s" s="13">
-        <v>18</v>
-      </c>
-      <c r="H10" t="s" s="13">
+      <c r="D10" t="s" s="27">
         <v>20</v>
       </c>
-      <c r="I10" t="s" s="13">
-        <v>18</v>
-      </c>
-      <c r="J10" t="s" s="13">
+      <c r="E10" t="s" s="27">
         <v>21</v>
       </c>
-      <c r="K10" t="s" s="13">
+      <c r="F10" t="s" s="27">
         <v>22</v>
       </c>
-      <c r="L10" t="s" s="13">
+      <c r="G10" t="s" s="27">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s" s="27">
         <v>23</v>
       </c>
+      <c r="I10" t="s" s="27">
+        <v>21</v>
+      </c>
+      <c r="J10" t="s" s="27">
+        <v>24</v>
+      </c>
+      <c r="K10" t="s" s="27">
+        <v>25</v>
+      </c>
+      <c r="L10" t="s" s="27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" ht="13.55" customHeight="1">
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1867,84 +2122,413 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12" style="27" customWidth="1"/>
-    <col min="2" max="5" width="8.85156" style="27" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="27" customWidth="1"/>
+    <col min="1" max="1" width="12" style="42" customWidth="1"/>
+    <col min="2" max="5" width="8.85156" style="42" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" s="28"/>
-      <c r="B1" t="s" s="13">
-        <v>25</v>
-      </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="A1" s="43"/>
+      <c r="B1" t="s" s="27">
+        <v>27</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" ht="26.55" customHeight="1">
-      <c r="A2" t="s" s="21">
-        <v>26</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="A2" t="s" s="35">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s" s="27">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s" s="27">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s" s="27">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s" s="27">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="12" style="47" customWidth="1"/>
+    <col min="2" max="5" width="8.85156" style="47" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="47" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" s="43"/>
+      <c r="B1" t="s" s="27">
+        <v>27</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+    </row>
+    <row r="2" ht="26.55" customHeight="1">
+      <c r="A2" t="s" s="35">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s" s="27">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s" s="27">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s" s="27">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s" s="27">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="46"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="46"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="12" style="48" customWidth="1"/>
+    <col min="2" max="5" width="8.85156" style="48" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="48" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" s="43"/>
+      <c r="B1" t="s" s="27">
+        <v>27</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+    </row>
+    <row r="2" ht="26.55" customHeight="1">
+      <c r="A2" t="s" s="35">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s" s="27">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s" s="27">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s" s="27">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s" s="27">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="46"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="46"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="12" style="49" customWidth="1"/>
+    <col min="2" max="5" width="8.85156" style="49" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="49" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" s="43"/>
+      <c r="B1" t="s" s="27">
+        <v>27</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+    </row>
+    <row r="2" ht="26.55" customHeight="1">
+      <c r="A2" t="s" s="35">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s" s="27">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s" s="27">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s" s="27">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s" s="27">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="46"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="46"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>